<commit_message>
Test case , time log
</commit_message>
<xml_diff>
--- a/Improgress/4. Timelog/PM_TimeLog.xlsx
+++ b/Improgress/4. Timelog/PM_TimeLog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Capstone-Project\Improgress\4. Timelog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\Capstone-Project\Improgress\4. Timelog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68C7452-55CC-4430-89D8-6B83C6933B69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D977B4F-A142-4D17-89EC-2A7FBA2FA925}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Anh Minh" sheetId="14" r:id="rId5"/>
     <sheet name="Như Phương" sheetId="15" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="188">
   <si>
     <t>Work in period</t>
   </si>
@@ -490,15 +492,149 @@
   </si>
   <si>
     <t>DE_BusinessRule_V1.0, DE_MessageList_V1.0</t>
+  </si>
+  <si>
+    <t>Meeting_Mentor_14/10/2019
+Meeting-customer_18/10/2019</t>
+  </si>
+  <si>
+    <t>Meeting_Mentor_23/10/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research GIS , 
+prepare question for customer 
+Test plan </t>
+  </si>
+  <si>
+    <t>28/10/2019</t>
+  </si>
+  <si>
+    <t>29/10/2019</t>
+  </si>
+  <si>
+    <t>30/10/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test plan </t>
+  </si>
+  <si>
+    <t>31/10/2019</t>
+  </si>
+  <si>
+    <t>TE_Testplan_ver1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research React </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete the meeting minutes ; 
+Requiment plan </t>
+  </si>
+  <si>
+    <t>Meeting_Customer_29/10/2019
+Meeting_Mentor _30/10/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requiment plan </t>
+  </si>
+  <si>
+    <t>RE_RequimentPlan_ver1.0</t>
+  </si>
+  <si>
+    <t>Requiment process</t>
+  </si>
+  <si>
+    <t>RE_RequimentProcess_ver1.0</t>
+  </si>
+  <si>
+    <t>Test Process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete the meeting minutes ; 
+Review document ,  test process </t>
+  </si>
+  <si>
+    <t>TE_Testprocess_ver1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete the meeting minutes ;
+Review document 
+Analyst Requirement </t>
+  </si>
+  <si>
+    <t>Meeting_customer 8/10/2019
+Meeting_mentor 6/10/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ConOP document </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usecase Decription </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prepare EOMP #1 
+Update document </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Present EOMP1 
+Complete the meeting minutes 
+Report document for customer </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Complete the meeting minutes 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete RE document </t>
+  </si>
+  <si>
+    <t>Architure Driver</t>
+  </si>
+  <si>
+    <t>Update ConOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review document  
+Complete the meeting minutes 
+</t>
+  </si>
+  <si>
+    <t>Context Diagram</t>
+  </si>
+  <si>
+    <t>Architure Design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Complete the meeting minutes 
+Review document 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detail Design </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEst Case </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Case </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-1010000]d/m/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="mm/dd/yyyy;@"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -602,7 +738,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -961,6 +1097,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -975,7 +1156,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1151,11 +1332,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1169,6 +1347,12 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1178,9 +1362,28 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
@@ -2125,10 +2328,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3586,13 +3789,13 @@
       <c r="A6" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="42">
-        <f>'Như Phương'!C11</f>
-        <v>27</v>
-      </c>
-      <c r="C6" s="42">
-        <f>'Như Phương'!C20</f>
-        <v>29</v>
+      <c r="B6" s="42" t="e">
+        <f>'Như Phương'!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C6" s="42" t="e">
+        <f>'Như Phương'!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="D6" s="42"/>
       <c r="E6" s="43"/>
@@ -3629,159 +3832,159 @@
       <c r="AJ6" s="44"/>
       <c r="AK6" s="44"/>
       <c r="AL6" s="44"/>
-      <c r="AM6" s="35">
+      <c r="AM6" s="35" t="e">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="7" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="12">
+      <c r="B7" s="12" t="e">
         <f>SUM(B2:B6)</f>
-        <v>133.5</v>
-      </c>
-      <c r="C7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="C7" s="12" t="e">
         <f t="shared" ref="C7:R7" si="1">SUM(C2:C6)+B7</f>
-        <v>260</v>
-      </c>
-      <c r="D7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="D7" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>260</v>
-      </c>
-      <c r="E7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="E7" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>260</v>
-      </c>
-      <c r="F7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="F7" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>260</v>
-      </c>
-      <c r="G7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="G7" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>260</v>
-      </c>
-      <c r="H7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="H7" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>260</v>
-      </c>
-      <c r="I7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="I7" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>260</v>
-      </c>
-      <c r="J7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="J7" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>260</v>
-      </c>
-      <c r="K7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="K7" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>260</v>
-      </c>
-      <c r="L7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="L7" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>260</v>
-      </c>
-      <c r="M7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="M7" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>260</v>
-      </c>
-      <c r="N7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="N7" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>260</v>
-      </c>
-      <c r="O7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="O7" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>260</v>
-      </c>
-      <c r="P7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="P7" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>260</v>
-      </c>
-      <c r="Q7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="Q7" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>260</v>
-      </c>
-      <c r="R7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="R7" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>260</v>
-      </c>
-      <c r="S7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="S7" s="12" t="e">
         <f t="shared" ref="S7" si="2">SUM(S2:S6)+R7</f>
-        <v>260</v>
-      </c>
-      <c r="T7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="T7" s="12" t="e">
         <f t="shared" ref="T7" si="3">SUM(T2:T6)+S7</f>
-        <v>260</v>
-      </c>
-      <c r="U7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="U7" s="12" t="e">
         <f t="shared" ref="U7" si="4">SUM(U2:U6)+T7</f>
-        <v>260</v>
-      </c>
-      <c r="V7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="V7" s="12" t="e">
         <f t="shared" ref="V7" si="5">SUM(V2:V6)+U7</f>
-        <v>260</v>
-      </c>
-      <c r="W7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="W7" s="12" t="e">
         <f t="shared" ref="W7" si="6">SUM(W2:W6)+V7</f>
-        <v>260</v>
-      </c>
-      <c r="X7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="X7" s="12" t="e">
         <f t="shared" ref="X7" si="7">SUM(X2:X6)+W7</f>
-        <v>260</v>
-      </c>
-      <c r="Y7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="Y7" s="12" t="e">
         <f t="shared" ref="Y7" si="8">SUM(Y2:Y6)+X7</f>
-        <v>260</v>
-      </c>
-      <c r="Z7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="Z7" s="12" t="e">
         <f t="shared" ref="Z7" si="9">SUM(Z2:Z6)+Y7</f>
-        <v>260</v>
-      </c>
-      <c r="AA7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AA7" s="12" t="e">
         <f t="shared" ref="AA7" si="10">SUM(AA2:AA6)+Z7</f>
-        <v>260</v>
-      </c>
-      <c r="AB7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AB7" s="12" t="e">
         <f t="shared" ref="AB7" si="11">SUM(AB2:AB6)+AA7</f>
-        <v>260</v>
-      </c>
-      <c r="AC7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AC7" s="12" t="e">
         <f t="shared" ref="AC7" si="12">SUM(AC2:AC6)+AB7</f>
-        <v>260</v>
-      </c>
-      <c r="AD7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AD7" s="12" t="e">
         <f t="shared" ref="AD7" si="13">SUM(AD2:AD6)+AC7</f>
-        <v>260</v>
-      </c>
-      <c r="AE7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AE7" s="12" t="e">
         <f t="shared" ref="AE7" si="14">SUM(AE2:AE6)+AD7</f>
-        <v>260</v>
-      </c>
-      <c r="AF7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AF7" s="12" t="e">
         <f t="shared" ref="AF7" si="15">SUM(AF2:AF6)+AE7</f>
-        <v>260</v>
-      </c>
-      <c r="AG7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AG7" s="12" t="e">
         <f t="shared" ref="AG7" si="16">SUM(AG2:AG6)+AF7</f>
-        <v>260</v>
-      </c>
-      <c r="AH7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AH7" s="12" t="e">
         <f t="shared" ref="AH7" si="17">SUM(AH2:AH6)+AG7</f>
-        <v>260</v>
-      </c>
-      <c r="AI7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AI7" s="12" t="e">
         <f t="shared" ref="AI7" si="18">SUM(AI2:AI6)+AH7</f>
-        <v>260</v>
-      </c>
-      <c r="AJ7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AJ7" s="12" t="e">
         <f t="shared" ref="AJ7" si="19">SUM(AJ2:AJ6)+AI7</f>
-        <v>260</v>
-      </c>
-      <c r="AK7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AK7" s="12" t="e">
         <f t="shared" ref="AK7" si="20">SUM(AK2:AK6)+AJ7</f>
-        <v>260</v>
-      </c>
-      <c r="AL7" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AL7" s="12" t="e">
         <f t="shared" ref="AL7" si="21">SUM(AL2:AL6)+AK7</f>
-        <v>260</v>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="8" spans="1:39" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4118,13 +4321,13 @@
       <c r="A13" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="B13" s="42">
-        <f>'Như Phương'!H11</f>
-        <v>28</v>
-      </c>
-      <c r="C13" s="42">
-        <f>'Như Phương'!H20</f>
-        <v>29</v>
+      <c r="B13" s="42" t="e">
+        <f>'Như Phương'!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C13" s="42" t="e">
+        <f>'Như Phương'!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="D13" s="41"/>
       <c r="E13" s="54"/>
@@ -4161,159 +4364,159 @@
       <c r="AJ13" s="41"/>
       <c r="AK13" s="41"/>
       <c r="AL13" s="41"/>
-      <c r="AM13" s="48">
+      <c r="AM13" s="48" t="e">
         <f t="shared" si="22"/>
-        <v>57</v>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="B14" s="12">
+      <c r="B14" s="12" t="e">
         <f>SUM(B9:B13)</f>
-        <v>139.5</v>
-      </c>
-      <c r="C14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="C14" s="12" t="e">
         <f t="shared" ref="C14:R14" si="23">SUM(C9:C13)+B14</f>
-        <v>284.5</v>
-      </c>
-      <c r="D14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="D14" s="12" t="e">
         <f t="shared" si="23"/>
-        <v>322.5</v>
-      </c>
-      <c r="E14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="E14" s="12" t="e">
         <f t="shared" si="23"/>
-        <v>322.5</v>
-      </c>
-      <c r="F14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="F14" s="12" t="e">
         <f t="shared" si="23"/>
-        <v>322.5</v>
-      </c>
-      <c r="G14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="G14" s="12" t="e">
         <f t="shared" si="23"/>
-        <v>322.5</v>
-      </c>
-      <c r="H14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="H14" s="12" t="e">
         <f t="shared" si="23"/>
-        <v>322.5</v>
-      </c>
-      <c r="I14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="I14" s="12" t="e">
         <f t="shared" si="23"/>
-        <v>322.5</v>
-      </c>
-      <c r="J14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="J14" s="12" t="e">
         <f t="shared" si="23"/>
-        <v>322.5</v>
-      </c>
-      <c r="K14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="K14" s="12" t="e">
         <f t="shared" si="23"/>
-        <v>322.5</v>
-      </c>
-      <c r="L14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="L14" s="12" t="e">
         <f t="shared" si="23"/>
-        <v>322.5</v>
-      </c>
-      <c r="M14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="M14" s="12" t="e">
         <f t="shared" si="23"/>
-        <v>322.5</v>
-      </c>
-      <c r="N14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="N14" s="12" t="e">
         <f t="shared" si="23"/>
-        <v>322.5</v>
-      </c>
-      <c r="O14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="O14" s="12" t="e">
         <f t="shared" si="23"/>
-        <v>322.5</v>
-      </c>
-      <c r="P14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="P14" s="12" t="e">
         <f t="shared" si="23"/>
-        <v>322.5</v>
-      </c>
-      <c r="Q14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="Q14" s="12" t="e">
         <f t="shared" si="23"/>
-        <v>322.5</v>
-      </c>
-      <c r="R14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="R14" s="12" t="e">
         <f t="shared" si="23"/>
-        <v>322.5</v>
-      </c>
-      <c r="S14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="S14" s="12" t="e">
         <f t="shared" ref="S14" si="24">SUM(S9:S13)+R14</f>
-        <v>322.5</v>
-      </c>
-      <c r="T14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="T14" s="12" t="e">
         <f t="shared" ref="T14" si="25">SUM(T9:T13)+S14</f>
-        <v>322.5</v>
-      </c>
-      <c r="U14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="U14" s="12" t="e">
         <f t="shared" ref="U14" si="26">SUM(U9:U13)+T14</f>
-        <v>322.5</v>
-      </c>
-      <c r="V14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="V14" s="12" t="e">
         <f t="shared" ref="V14" si="27">SUM(V9:V13)+U14</f>
-        <v>322.5</v>
-      </c>
-      <c r="W14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="W14" s="12" t="e">
         <f t="shared" ref="W14" si="28">SUM(W9:W13)+V14</f>
-        <v>322.5</v>
-      </c>
-      <c r="X14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="X14" s="12" t="e">
         <f t="shared" ref="X14" si="29">SUM(X9:X13)+W14</f>
-        <v>322.5</v>
-      </c>
-      <c r="Y14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="Y14" s="12" t="e">
         <f t="shared" ref="Y14" si="30">SUM(Y9:Y13)+X14</f>
-        <v>322.5</v>
-      </c>
-      <c r="Z14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="Z14" s="12" t="e">
         <f t="shared" ref="Z14" si="31">SUM(Z9:Z13)+Y14</f>
-        <v>322.5</v>
-      </c>
-      <c r="AA14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AA14" s="12" t="e">
         <f t="shared" ref="AA14" si="32">SUM(AA9:AA13)+Z14</f>
-        <v>322.5</v>
-      </c>
-      <c r="AB14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AB14" s="12" t="e">
         <f t="shared" ref="AB14" si="33">SUM(AB9:AB13)+AA14</f>
-        <v>322.5</v>
-      </c>
-      <c r="AC14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AC14" s="12" t="e">
         <f t="shared" ref="AC14" si="34">SUM(AC9:AC13)+AB14</f>
-        <v>322.5</v>
-      </c>
-      <c r="AD14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AD14" s="12" t="e">
         <f t="shared" ref="AD14" si="35">SUM(AD9:AD13)+AC14</f>
-        <v>322.5</v>
-      </c>
-      <c r="AE14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AE14" s="12" t="e">
         <f t="shared" ref="AE14" si="36">SUM(AE9:AE13)+AD14</f>
-        <v>322.5</v>
-      </c>
-      <c r="AF14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AF14" s="12" t="e">
         <f t="shared" ref="AF14" si="37">SUM(AF9:AF13)+AE14</f>
-        <v>322.5</v>
-      </c>
-      <c r="AG14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AG14" s="12" t="e">
         <f t="shared" ref="AG14" si="38">SUM(AG9:AG13)+AF14</f>
-        <v>322.5</v>
-      </c>
-      <c r="AH14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AH14" s="12" t="e">
         <f t="shared" ref="AH14" si="39">SUM(AH9:AH13)+AG14</f>
-        <v>322.5</v>
-      </c>
-      <c r="AI14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AI14" s="12" t="e">
         <f t="shared" ref="AI14" si="40">SUM(AI9:AI13)+AH14</f>
-        <v>322.5</v>
-      </c>
-      <c r="AJ14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AJ14" s="12" t="e">
         <f t="shared" ref="AJ14" si="41">SUM(AJ9:AJ13)+AI14</f>
-        <v>322.5</v>
-      </c>
-      <c r="AK14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AK14" s="12" t="e">
         <f t="shared" ref="AK14" si="42">SUM(AK9:AK13)+AJ14</f>
-        <v>322.5</v>
-      </c>
-      <c r="AL14" s="12">
+        <v>#REF!</v>
+      </c>
+      <c r="AL14" s="12" t="e">
         <f t="shared" ref="AL14" si="43">SUM(AL9:AL13)+AK14</f>
-        <v>322.5</v>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>
@@ -4361,17 +4564,17 @@
       <c r="I1" s="22"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="74"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
@@ -4578,21 +4781,21 @@
       <c r="B11" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="69">
+      <c r="C11" s="74">
         <f>SUM(F4:F10)</f>
         <v>30</v>
       </c>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="75"/>
       <c r="G11" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="69">
+      <c r="H11" s="74">
         <f>SUM(G4:G10)</f>
         <v>30</v>
       </c>
-      <c r="I11" s="70"/>
+      <c r="I11" s="75"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
@@ -4795,21 +4998,21 @@
       <c r="B20" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="69">
+      <c r="C20" s="74">
         <f>SUM(F13:F19)</f>
         <v>22</v>
       </c>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="70"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="75"/>
       <c r="G20" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="69">
+      <c r="H20" s="74">
         <f>SUM(G13:G19)</f>
         <v>34</v>
       </c>
-      <c r="I20" s="70"/>
+      <c r="I20" s="75"/>
     </row>
     <row r="21" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
@@ -5016,21 +5219,21 @@
       <c r="B30" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="69">
+      <c r="C30" s="74">
         <f>SUM(F22:F29)</f>
         <v>0</v>
       </c>
-      <c r="D30" s="69"/>
-      <c r="E30" s="69"/>
-      <c r="F30" s="70"/>
+      <c r="D30" s="74"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="75"/>
       <c r="G30" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H30" s="69">
+      <c r="H30" s="74">
         <f>SUM(G22:G29)</f>
         <v>38</v>
       </c>
-      <c r="I30" s="70"/>
+      <c r="I30" s="75"/>
     </row>
     <row r="31" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
@@ -5184,21 +5387,21 @@
       <c r="B39" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C39" s="69">
+      <c r="C39" s="74">
         <f>SUM(F32:F38)</f>
         <v>0</v>
       </c>
-      <c r="D39" s="69"/>
-      <c r="E39" s="69"/>
-      <c r="F39" s="70"/>
+      <c r="D39" s="74"/>
+      <c r="E39" s="74"/>
+      <c r="F39" s="75"/>
       <c r="G39" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H39" s="69">
+      <c r="H39" s="74">
         <f>SUM(G32:G38)</f>
         <v>0</v>
       </c>
-      <c r="I39" s="70"/>
+      <c r="I39" s="75"/>
     </row>
     <row r="40" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
@@ -5348,21 +5551,21 @@
       <c r="B48" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="69">
+      <c r="C48" s="74">
         <f>SUM(F41:F47)</f>
         <v>0</v>
       </c>
-      <c r="D48" s="69"/>
-      <c r="E48" s="69"/>
-      <c r="F48" s="70"/>
+      <c r="D48" s="74"/>
+      <c r="E48" s="74"/>
+      <c r="F48" s="75"/>
       <c r="G48" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H48" s="69">
+      <c r="H48" s="74">
         <f>SUM(G41:G47)</f>
         <v>0</v>
       </c>
-      <c r="I48" s="70"/>
+      <c r="I48" s="75"/>
     </row>
     <row r="49" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="24" t="s">
@@ -5512,21 +5715,21 @@
       <c r="B57" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C57" s="69">
+      <c r="C57" s="74">
         <f>SUM(F50:F56)</f>
         <v>0</v>
       </c>
-      <c r="D57" s="69"/>
-      <c r="E57" s="69"/>
-      <c r="F57" s="70"/>
+      <c r="D57" s="74"/>
+      <c r="E57" s="74"/>
+      <c r="F57" s="75"/>
       <c r="G57" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H57" s="69">
+      <c r="H57" s="74">
         <f>SUM(G50:G56)</f>
         <v>0</v>
       </c>
-      <c r="I57" s="70"/>
+      <c r="I57" s="75"/>
     </row>
     <row r="58" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="24" t="s">
@@ -5676,24 +5879,30 @@
       <c r="B66" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C66" s="69">
+      <c r="C66" s="74">
         <f>SUM(F59:F65)</f>
         <v>0</v>
       </c>
-      <c r="D66" s="69"/>
-      <c r="E66" s="69"/>
-      <c r="F66" s="70"/>
+      <c r="D66" s="74"/>
+      <c r="E66" s="74"/>
+      <c r="F66" s="75"/>
       <c r="G66" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H66" s="69">
+      <c r="H66" s="74">
         <f>SUM(G59:G65)</f>
         <v>0</v>
       </c>
-      <c r="I66" s="70"/>
+      <c r="I66" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C66:F66"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="H20:I20"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="C48:F48"/>
     <mergeCell ref="H48:I48"/>
@@ -5703,12 +5912,6 @@
     <mergeCell ref="H30:I30"/>
     <mergeCell ref="C39:F39"/>
     <mergeCell ref="H39:I39"/>
-    <mergeCell ref="C66:F66"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="H20:I20"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="6">
@@ -5743,7 +5946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B58" workbookViewId="0">
+    <sheetView topLeftCell="B58" workbookViewId="0">
       <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
@@ -5774,17 +5977,17 @@
       <c r="I1" s="22"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="74"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
@@ -5991,21 +6194,21 @@
       <c r="B11" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="75">
+      <c r="C11" s="76">
         <f>SUM(F4:F10)</f>
         <v>26</v>
       </c>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="75"/>
       <c r="G11" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="69">
+      <c r="H11" s="74">
         <f>SUM(G4:G10)</f>
         <v>26</v>
       </c>
-      <c r="I11" s="70"/>
+      <c r="I11" s="75"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
@@ -6218,21 +6421,21 @@
       <c r="B20" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="69">
+      <c r="C20" s="74">
         <f>SUM(F13:F19)</f>
         <v>30</v>
       </c>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="70"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="75"/>
       <c r="G20" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="69">
+      <c r="H20" s="74">
         <f>SUM(G13:G19)</f>
         <v>30</v>
       </c>
-      <c r="I20" s="70"/>
+      <c r="I20" s="75"/>
     </row>
     <row r="21" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
@@ -6273,7 +6476,7 @@
       <c r="C22" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="78" t="s">
+      <c r="D22" s="69" t="s">
         <v>118</v>
       </c>
       <c r="E22" s="18">
@@ -6298,7 +6501,7 @@
       <c r="C23" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="78" t="s">
+      <c r="D23" s="69" t="s">
         <v>119</v>
       </c>
       <c r="E23" s="18">
@@ -6451,21 +6654,21 @@
       <c r="B29" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="69">
+      <c r="C29" s="74">
         <f>SUM(F22:F28)</f>
         <v>45</v>
       </c>
-      <c r="D29" s="69"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="70"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="75"/>
       <c r="G29" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H29" s="69">
+      <c r="H29" s="74">
         <f>SUM(G22:G28)</f>
         <v>0</v>
       </c>
-      <c r="I29" s="70"/>
+      <c r="I29" s="75"/>
     </row>
     <row r="30" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="24" t="s">
@@ -6506,7 +6709,7 @@
       <c r="C31" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="78" t="s">
+      <c r="D31" s="69" t="s">
         <v>128</v>
       </c>
       <c r="E31" s="18">
@@ -6660,21 +6863,21 @@
       <c r="B38" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="69">
+      <c r="C38" s="74">
         <f>SUM(F31:F37)</f>
         <v>38</v>
       </c>
-      <c r="D38" s="69"/>
-      <c r="E38" s="69"/>
-      <c r="F38" s="70"/>
+      <c r="D38" s="74"/>
+      <c r="E38" s="74"/>
+      <c r="F38" s="75"/>
       <c r="G38" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H38" s="69">
+      <c r="H38" s="74">
         <f>SUM(G31:G37)</f>
         <v>0</v>
       </c>
-      <c r="I38" s="70"/>
+      <c r="I38" s="75"/>
     </row>
     <row r="39" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="24" t="s">
@@ -6827,21 +7030,21 @@
       <c r="B47" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="69">
+      <c r="C47" s="74">
         <f>SUM(F40:F46)</f>
         <v>0</v>
       </c>
-      <c r="D47" s="69"/>
-      <c r="E47" s="69"/>
-      <c r="F47" s="70"/>
+      <c r="D47" s="74"/>
+      <c r="E47" s="74"/>
+      <c r="F47" s="75"/>
       <c r="G47" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H47" s="69">
+      <c r="H47" s="74">
         <f>SUM(G40:G46)</f>
         <v>0</v>
       </c>
-      <c r="I47" s="70"/>
+      <c r="I47" s="75"/>
     </row>
     <row r="48" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="24" t="s">
@@ -6994,21 +7197,21 @@
       <c r="B56" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C56" s="69">
+      <c r="C56" s="74">
         <f>SUM(F49:F55)</f>
         <v>0</v>
       </c>
-      <c r="D56" s="69"/>
-      <c r="E56" s="69"/>
-      <c r="F56" s="70"/>
+      <c r="D56" s="74"/>
+      <c r="E56" s="74"/>
+      <c r="F56" s="75"/>
       <c r="G56" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H56" s="69">
+      <c r="H56" s="74">
         <f>SUM(G49:G55)</f>
         <v>0</v>
       </c>
-      <c r="I56" s="70"/>
+      <c r="I56" s="75"/>
     </row>
     <row r="57" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="24" t="s">
@@ -7217,21 +7420,21 @@
       <c r="B65" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C65" s="69">
+      <c r="C65" s="74">
         <f>SUM(F58:F64)</f>
         <v>50</v>
       </c>
-      <c r="D65" s="69"/>
-      <c r="E65" s="69"/>
-      <c r="F65" s="70"/>
+      <c r="D65" s="74"/>
+      <c r="E65" s="74"/>
+      <c r="F65" s="75"/>
       <c r="G65" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H65" s="69">
+      <c r="H65" s="74">
         <f>SUM(G58:G64)</f>
         <v>0</v>
       </c>
-      <c r="I65" s="70"/>
+      <c r="I65" s="75"/>
     </row>
     <row r="66" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="24" t="s">
@@ -7408,35 +7611,35 @@
       <c r="B74" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C74" s="69">
+      <c r="C74" s="74">
         <f>SUM(F67:F73)</f>
         <v>10</v>
       </c>
-      <c r="D74" s="69"/>
-      <c r="E74" s="69"/>
-      <c r="F74" s="70"/>
+      <c r="D74" s="74"/>
+      <c r="E74" s="74"/>
+      <c r="F74" s="75"/>
       <c r="G74" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H74" s="69">
+      <c r="H74" s="74">
         <f>SUM(G67:G73)</f>
         <v>0</v>
       </c>
-      <c r="I74" s="70"/>
+      <c r="I74" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="H20:I20"/>
     <mergeCell ref="C74:F74"/>
     <mergeCell ref="H74:I74"/>
     <mergeCell ref="C65:F65"/>
     <mergeCell ref="H65:I65"/>
     <mergeCell ref="C29:F29"/>
     <mergeCell ref="H29:I29"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="H20:I20"/>
     <mergeCell ref="C38:F38"/>
     <mergeCell ref="H38:I38"/>
     <mergeCell ref="C47:F47"/>
@@ -7505,17 +7708,17 @@
       <c r="I1" s="22"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="74"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
@@ -7720,21 +7923,21 @@
       <c r="B11" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="76">
+      <c r="C11" s="77">
         <f>SUM(F4:F10)</f>
         <v>26.5</v>
       </c>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="77"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="78"/>
       <c r="G11" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="76">
+      <c r="H11" s="77">
         <f>SUM(G4:G10)</f>
         <v>27.5</v>
       </c>
-      <c r="I11" s="77"/>
+      <c r="I11" s="78"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
@@ -7935,21 +8138,21 @@
       <c r="B20" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="76">
+      <c r="C20" s="77">
         <f>SUM(F13:F19)</f>
         <v>18.5</v>
       </c>
-      <c r="D20" s="76"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="77"/>
+      <c r="D20" s="77"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="78"/>
       <c r="G20" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="76">
+      <c r="H20" s="77">
         <f>SUM(G13:G19)</f>
         <v>22</v>
       </c>
-      <c r="I20" s="77"/>
+      <c r="I20" s="78"/>
     </row>
     <row r="21" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
@@ -8088,21 +8291,21 @@
       <c r="B29" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="69">
+      <c r="C29" s="74">
         <f>SUM(F22:F28)</f>
         <v>0</v>
       </c>
-      <c r="D29" s="69"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="70"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="75"/>
       <c r="G29" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H29" s="69">
+      <c r="H29" s="74">
         <f>SUM(G22:G28)</f>
         <v>0</v>
       </c>
-      <c r="I29" s="70"/>
+      <c r="I29" s="75"/>
     </row>
     <row r="30" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="24" t="s">
@@ -8241,21 +8444,21 @@
       <c r="B38" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="69">
+      <c r="C38" s="74">
         <f>SUM(F31:F37)</f>
         <v>0</v>
       </c>
-      <c r="D38" s="69"/>
-      <c r="E38" s="69"/>
-      <c r="F38" s="70"/>
+      <c r="D38" s="74"/>
+      <c r="E38" s="74"/>
+      <c r="F38" s="75"/>
       <c r="G38" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H38" s="69">
+      <c r="H38" s="74">
         <f>SUM(G31:G37)</f>
         <v>0</v>
       </c>
-      <c r="I38" s="70"/>
+      <c r="I38" s="75"/>
     </row>
     <row r="39" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="24" t="s">
@@ -8394,21 +8597,21 @@
       <c r="B47" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="69">
+      <c r="C47" s="74">
         <f>SUM(F40:F46)</f>
         <v>0</v>
       </c>
-      <c r="D47" s="69"/>
-      <c r="E47" s="69"/>
-      <c r="F47" s="70"/>
+      <c r="D47" s="74"/>
+      <c r="E47" s="74"/>
+      <c r="F47" s="75"/>
       <c r="G47" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H47" s="69">
+      <c r="H47" s="74">
         <f>SUM(G40:G46)</f>
         <v>0</v>
       </c>
-      <c r="I47" s="70"/>
+      <c r="I47" s="75"/>
     </row>
     <row r="48" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="24" t="s">
@@ -8547,24 +8750,29 @@
       <c r="B56" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C56" s="69">
+      <c r="C56" s="74">
         <f>SUM(F49:F55)</f>
         <v>0</v>
       </c>
-      <c r="D56" s="69"/>
-      <c r="E56" s="69"/>
-      <c r="F56" s="70"/>
+      <c r="D56" s="74"/>
+      <c r="E56" s="74"/>
+      <c r="F56" s="75"/>
       <c r="G56" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H56" s="69">
+      <c r="H56" s="74">
         <f>SUM(G49:G55)</f>
         <v>0</v>
       </c>
-      <c r="I56" s="70"/>
+      <c r="I56" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="H20:I20"/>
     <mergeCell ref="C56:F56"/>
     <mergeCell ref="H56:I56"/>
     <mergeCell ref="C29:F29"/>
@@ -8573,11 +8781,6 @@
     <mergeCell ref="H38:I38"/>
     <mergeCell ref="C47:F47"/>
     <mergeCell ref="H47:I47"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="H20:I20"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 B12" xr:uid="{6FFE7BB2-A561-485E-81E9-2571AC8DE5CA}">
@@ -8639,17 +8842,17 @@
       <c r="I1" s="22"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="74"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
@@ -8854,21 +9057,21 @@
       <c r="B11" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="76">
+      <c r="C11" s="77">
         <f>SUM(F4:F10)</f>
         <v>24</v>
       </c>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="77"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="78"/>
       <c r="G11" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="76">
+      <c r="H11" s="77">
         <f>SUM(G4:G10)</f>
         <v>28</v>
       </c>
-      <c r="I11" s="77"/>
+      <c r="I11" s="78"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
@@ -9077,21 +9280,21 @@
       <c r="B20" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="76">
+      <c r="C20" s="77">
         <f>SUM(F13:F19)</f>
         <v>27</v>
       </c>
-      <c r="D20" s="76"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="77"/>
+      <c r="D20" s="77"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="78"/>
       <c r="G20" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="76">
+      <c r="H20" s="77">
         <f>SUM(G13:G19)</f>
         <v>30</v>
       </c>
-      <c r="I20" s="77"/>
+      <c r="I20" s="78"/>
     </row>
     <row r="21" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
@@ -9230,21 +9433,21 @@
       <c r="B29" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="69">
+      <c r="C29" s="74">
         <f>SUM(F22:F28)</f>
         <v>0</v>
       </c>
-      <c r="D29" s="69"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="70"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="75"/>
       <c r="G29" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H29" s="69">
+      <c r="H29" s="74">
         <f>SUM(G22:G28)</f>
         <v>0</v>
       </c>
-      <c r="I29" s="70"/>
+      <c r="I29" s="75"/>
     </row>
     <row r="30" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="24" t="s">
@@ -9383,21 +9586,21 @@
       <c r="B38" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="69">
+      <c r="C38" s="74">
         <f>SUM(F31:F37)</f>
         <v>0</v>
       </c>
-      <c r="D38" s="69"/>
-      <c r="E38" s="69"/>
-      <c r="F38" s="70"/>
+      <c r="D38" s="74"/>
+      <c r="E38" s="74"/>
+      <c r="F38" s="75"/>
       <c r="G38" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H38" s="69">
+      <c r="H38" s="74">
         <f>SUM(G31:G37)</f>
         <v>0</v>
       </c>
-      <c r="I38" s="70"/>
+      <c r="I38" s="75"/>
     </row>
     <row r="39" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="24" t="s">
@@ -9536,21 +9739,21 @@
       <c r="B47" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="69">
+      <c r="C47" s="74">
         <f>SUM(F40:F46)</f>
         <v>0</v>
       </c>
-      <c r="D47" s="69"/>
-      <c r="E47" s="69"/>
-      <c r="F47" s="70"/>
+      <c r="D47" s="74"/>
+      <c r="E47" s="74"/>
+      <c r="F47" s="75"/>
       <c r="G47" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H47" s="69">
+      <c r="H47" s="74">
         <f>SUM(G40:G46)</f>
         <v>0</v>
       </c>
-      <c r="I47" s="70"/>
+      <c r="I47" s="75"/>
     </row>
     <row r="48" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="24" t="s">
@@ -9689,24 +9892,29 @@
       <c r="B56" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C56" s="69">
+      <c r="C56" s="74">
         <f>SUM(F49:F55)</f>
         <v>0</v>
       </c>
-      <c r="D56" s="69"/>
-      <c r="E56" s="69"/>
-      <c r="F56" s="70"/>
+      <c r="D56" s="74"/>
+      <c r="E56" s="74"/>
+      <c r="F56" s="75"/>
       <c r="G56" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H56" s="69">
+      <c r="H56" s="74">
         <f>SUM(G49:G55)</f>
         <v>0</v>
       </c>
-      <c r="I56" s="70"/>
+      <c r="I56" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="H20:I20"/>
     <mergeCell ref="C56:F56"/>
     <mergeCell ref="H56:I56"/>
     <mergeCell ref="C29:F29"/>
@@ -9715,11 +9923,6 @@
     <mergeCell ref="H38:I38"/>
     <mergeCell ref="C47:F47"/>
     <mergeCell ref="H47:I47"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="H20:I20"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C19 C28 C37 C46 C55" xr:uid="{49E4ABBA-BF99-4A08-9146-05B03FF61551}">
@@ -9751,10 +9954,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{744DDA93-81BE-4148-9787-FFABC05BF7AA}">
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:L75"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75:I75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9764,10 +9967,10 @@
     <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>65</v>
       </c>
@@ -9780,49 +9983,49 @@
       <c r="H1" s="21"/>
       <c r="I1" s="22"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="71" t="s">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="74"/>
-    </row>
-    <row r="3" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="71"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="73"/>
+    </row>
+    <row r="3" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="79" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="24" t="s">
+      <c r="F3" s="80" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="81" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>1</v>
       </c>
@@ -9847,7 +10050,7 @@
       </c>
       <c r="I4" s="15"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>1</v>
       </c>
@@ -9867,14 +10070,15 @@
         <v>5</v>
       </c>
       <c r="G5" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H5" s="14" t="s">
         <v>20</v>
       </c>
       <c r="I5" s="15"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L5" s="86"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -9894,14 +10098,14 @@
         <v>5</v>
       </c>
       <c r="G6" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H6" s="14" t="s">
         <v>20</v>
       </c>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -9928,7 +10132,7 @@
       </c>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -9953,7 +10157,7 @@
       </c>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -9978,9 +10182,11 @@
       <c r="H9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="82" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="11"/>
       <c r="C10" s="9"/>
@@ -9991,73 +10197,71 @@
       <c r="H10" s="14"/>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="67" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="76">
+      <c r="C11" s="77">
         <f>SUM(F4:F10)</f>
         <v>27</v>
       </c>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="77"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="78"/>
       <c r="G11" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="76">
+      <c r="H11" s="77">
         <f>SUM(G4:G10)</f>
-        <v>28</v>
-      </c>
-      <c r="I11" s="77"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="78"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
         <v>2</v>
       </c>
-      <c r="C12" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="24" t="s">
+      <c r="B12" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="56" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="10">
+        <v>5</v>
+      </c>
+      <c r="G12" s="10">
         <v>4</v>
       </c>
-      <c r="F12" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="I12" s="24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H12" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="15"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>2</v>
       </c>
-      <c r="B13" s="25" t="s">
-        <v>9</v>
+      <c r="B13" s="26" t="s">
+        <v>10</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="56" t="s">
-        <v>104</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>71</v>
+        <v>105</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>72</v>
       </c>
       <c r="F13" s="10">
         <v>5</v>
@@ -10070,64 +10274,64 @@
       </c>
       <c r="I13" s="15"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>2</v>
       </c>
-      <c r="B14" s="26" t="s">
-        <v>10</v>
+      <c r="B14" s="27" t="s">
+        <v>11</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="56" t="s">
-        <v>105</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" s="10">
-        <v>5</v>
-      </c>
-      <c r="G14" s="10">
+        <v>63</v>
+      </c>
+      <c r="D14" s="57"/>
+      <c r="E14" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="1">
+        <v>4</v>
+      </c>
+      <c r="G14" s="1">
         <v>5</v>
       </c>
       <c r="H14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="15"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>2</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="57"/>
-      <c r="E15" s="17" t="s">
-        <v>73</v>
+        <v>19</v>
+      </c>
+      <c r="D15" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>74</v>
       </c>
       <c r="F15" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G15" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H15" s="14" t="s">
         <v>20</v>
       </c>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>2</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C16" s="25" t="s">
         <v>19</v>
@@ -10135,8 +10339,8 @@
       <c r="D16" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="E16" s="19" t="s">
-        <v>74</v>
+      <c r="E16" s="16" t="s">
+        <v>76</v>
       </c>
       <c r="F16" s="1">
         <v>5</v>
@@ -10149,743 +10353,1408 @@
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>2</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C17" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="57" t="s">
-        <v>106</v>
+      <c r="D17" s="63" t="s">
+        <v>107</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="F17" s="1">
         <v>5</v>
       </c>
       <c r="G17" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H17" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
-        <v>2</v>
-      </c>
-      <c r="B18" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="25" t="s">
+      <c r="I17" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="77">
+        <f>SUM(F12:F18)</f>
+        <v>29</v>
+      </c>
+      <c r="D19" s="77"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="66" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="77">
+        <f>SUM(G12:G18)</f>
+        <v>30</v>
+      </c>
+      <c r="I19" s="78"/>
+    </row>
+    <row r="20" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10">
+        <v>3</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="63" t="s">
-        <v>107</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="F18" s="1">
-        <v>5</v>
-      </c>
-      <c r="G18" s="1">
-        <v>5</v>
-      </c>
-      <c r="H18" s="14" t="s">
+      <c r="D20" s="69" t="s">
+        <v>152</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="F20" s="10">
+        <v>5.5</v>
+      </c>
+      <c r="G20" s="10">
+        <v>6</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="15"/>
+    </row>
+    <row r="21" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="10">
+        <v>3</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="56"/>
+      <c r="E21" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="F21" s="10">
+        <v>4</v>
+      </c>
+      <c r="G21" s="10">
+        <v>5</v>
+      </c>
+      <c r="H21" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="67" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="76">
-        <f>SUM(F13:F19)</f>
-        <v>29</v>
-      </c>
-      <c r="D20" s="76"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="77"/>
-      <c r="G20" s="66" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" s="76">
-        <f>SUM(G13:G19)</f>
-        <v>29</v>
-      </c>
-      <c r="I20" s="77"/>
-    </row>
-    <row r="21" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I21" s="15"/>
+    </row>
+    <row r="22" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10">
         <v>3</v>
       </c>
-      <c r="B22" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="25"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="15"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="57"/>
+      <c r="E22" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="F22" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G22" s="1">
+        <v>5</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10">
         <v>3</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="25"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="15"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="57" t="s">
+        <v>156</v>
+      </c>
+      <c r="E23" s="83" t="s">
+        <v>157</v>
+      </c>
+      <c r="F23" s="1">
+        <v>5</v>
+      </c>
+      <c r="G23" s="1">
+        <v>6</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10">
         <v>3</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="14"/>
+        <v>13</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="57" t="s">
+        <v>159</v>
+      </c>
+      <c r="E24" s="83">
+        <v>43476</v>
+      </c>
+      <c r="F24" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G24" s="1">
+        <v>6</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>20</v>
+      </c>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>3</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
-        <v>3</v>
-      </c>
-      <c r="B26" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="63" t="s">
+        <v>160</v>
+      </c>
+      <c r="E25" s="83">
+        <v>43507</v>
+      </c>
+      <c r="F25" s="1">
+        <v>6</v>
+      </c>
+      <c r="G25" s="1">
+        <v>7</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" s="82" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="9"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="59"/>
       <c r="E26" s="16"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
       <c r="H26" s="14"/>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
-        <v>3</v>
-      </c>
-      <c r="B27" s="68" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="25"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="5"/>
-    </row>
-    <row r="29" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="67" t="s">
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="67" t="s">
+      <c r="B27" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="69">
-        <f>SUM(F22:F28)</f>
-        <v>0</v>
-      </c>
-      <c r="D29" s="69"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="70"/>
-      <c r="G29" s="66" t="s">
+      <c r="C27" s="77">
+        <f>SUM(F20:F26)</f>
+        <v>29.5</v>
+      </c>
+      <c r="D27" s="77"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="78"/>
+      <c r="G27" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="H29" s="69">
-        <f>SUM(G22:G28)</f>
-        <v>0</v>
-      </c>
-      <c r="I29" s="70"/>
+      <c r="H27" s="77">
+        <f>SUM(G20:G26)</f>
+        <v>35</v>
+      </c>
+      <c r="I27" s="78"/>
+    </row>
+    <row r="28" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="10">
+        <v>4</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="69" t="s">
+        <v>162</v>
+      </c>
+      <c r="E28" s="18">
+        <v>43773</v>
+      </c>
+      <c r="F28" s="10">
+        <v>5.5</v>
+      </c>
+      <c r="G28" s="10">
+        <v>7</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="15" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="10">
+        <v>4</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="E29" s="18">
+        <v>43774</v>
+      </c>
+      <c r="F29" s="10">
+        <v>5</v>
+      </c>
+      <c r="G29" s="10">
+        <v>6</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" s="15" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="E30" s="24" t="s">
+      <c r="A30" s="10">
         <v>4</v>
       </c>
-      <c r="F30" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="G30" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="H30" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="I30" s="24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="57"/>
+      <c r="E30" s="18">
+        <v>43775</v>
+      </c>
+      <c r="F30" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G30" s="1">
+        <v>5</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10">
         <v>4</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="15"/>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="57" t="s">
+        <v>166</v>
+      </c>
+      <c r="E31" s="18">
+        <v>43776</v>
+      </c>
+      <c r="F31" s="1">
+        <v>5</v>
+      </c>
+      <c r="G31" s="1">
+        <v>7</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10">
         <v>4</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="25"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="15"/>
-    </row>
-    <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="57"/>
+      <c r="E32" s="18">
+        <v>43777</v>
+      </c>
+      <c r="F32" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G32" s="1">
+        <v>5</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>4</v>
       </c>
       <c r="B33" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="63" t="s">
+        <v>167</v>
+      </c>
+      <c r="E33" s="18">
+        <v>43778</v>
+      </c>
+      <c r="F33" s="1">
+        <v>7</v>
+      </c>
+      <c r="G33" s="1">
+        <v>5</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="9"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="77">
+        <f>SUM(F28:F34)</f>
+        <v>31.5</v>
+      </c>
+      <c r="D35" s="77"/>
+      <c r="E35" s="77"/>
+      <c r="F35" s="78"/>
+      <c r="G35" s="66" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" s="77">
+        <f>SUM(G28:G34)</f>
+        <v>35</v>
+      </c>
+      <c r="I35" s="78"/>
+    </row>
+    <row r="36" spans="1:9" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="10">
+        <v>5</v>
+      </c>
+      <c r="B36" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="69" t="s">
+        <v>169</v>
+      </c>
+      <c r="E36" s="18">
+        <v>43773</v>
+      </c>
+      <c r="F36" s="10">
+        <v>6</v>
+      </c>
+      <c r="G36" s="10"/>
+      <c r="H36" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I36" s="15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="10">
+        <v>5</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="56"/>
+      <c r="E37" s="18">
+        <v>43774</v>
+      </c>
+      <c r="F37" s="10">
+        <v>4</v>
+      </c>
+      <c r="G37" s="10"/>
+      <c r="H37" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I37" s="15"/>
+    </row>
+    <row r="38" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="10">
+        <v>5</v>
+      </c>
+      <c r="B38" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="3"/>
-    </row>
-    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="10">
+      <c r="C38" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="57" t="s">
+        <v>171</v>
+      </c>
+      <c r="E38" s="18">
+        <v>43775</v>
+      </c>
+      <c r="F38" s="1">
+        <v>5</v>
+      </c>
+      <c r="G38" s="10"/>
+      <c r="H38" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I38" s="3"/>
+    </row>
+    <row r="39" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="10">
+        <v>5</v>
+      </c>
+      <c r="B39" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="57" t="s">
+        <v>172</v>
+      </c>
+      <c r="E39" s="18">
+        <v>43776</v>
+      </c>
+      <c r="F39" s="1">
+        <v>5</v>
+      </c>
+      <c r="G39" s="10"/>
+      <c r="H39" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I39" s="3"/>
+    </row>
+    <row r="40" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="10">
+        <v>5</v>
+      </c>
+      <c r="B40" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="63" t="s">
+        <v>173</v>
+      </c>
+      <c r="E40" s="18">
+        <v>43777</v>
+      </c>
+      <c r="F40" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G40" s="10"/>
+      <c r="H40" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I40" s="3"/>
+    </row>
+    <row r="41" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="10">
+        <v>5</v>
+      </c>
+      <c r="B41" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="63" t="s">
+        <v>174</v>
+      </c>
+      <c r="E41" s="18">
+        <v>43778</v>
+      </c>
+      <c r="F41" s="1">
+        <v>6</v>
+      </c>
+      <c r="G41" s="10"/>
+      <c r="H41" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I41" s="3"/>
+    </row>
+    <row r="42" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="9"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="77">
+        <f>SUM(F36:F42)</f>
+        <v>30.5</v>
+      </c>
+      <c r="D43" s="77"/>
+      <c r="E43" s="77"/>
+      <c r="F43" s="78"/>
+      <c r="G43" s="66" t="s">
+        <v>17</v>
+      </c>
+      <c r="H43" s="77">
+        <f>SUM(G36:G42)</f>
+        <v>0</v>
+      </c>
+      <c r="I43" s="78"/>
+    </row>
+    <row r="44" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="10">
+        <v>6</v>
+      </c>
+      <c r="B44" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="69"/>
+      <c r="E44" s="18">
+        <v>43780</v>
+      </c>
+      <c r="F44" s="10">
+        <v>6</v>
+      </c>
+      <c r="G44" s="10"/>
+      <c r="H44" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I44" s="15"/>
+    </row>
+    <row r="45" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="10">
+        <v>6</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" s="56"/>
+      <c r="E45" s="18">
+        <v>43781</v>
+      </c>
+      <c r="F45" s="10">
         <v>4</v>
       </c>
-      <c r="B34" s="27" t="s">
+      <c r="G45" s="10"/>
+      <c r="H45" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I45" s="15"/>
+    </row>
+    <row r="46" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="10">
+        <v>6</v>
+      </c>
+      <c r="B46" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" s="57"/>
+      <c r="E46" s="18">
+        <v>43782</v>
+      </c>
+      <c r="F46" s="1">
+        <v>5</v>
+      </c>
+      <c r="G46" s="10"/>
+      <c r="H46" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I46" s="3"/>
+    </row>
+    <row r="47" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="10">
+        <v>6</v>
+      </c>
+      <c r="B47" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="25"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="3"/>
-    </row>
-    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="10">
-        <v>4</v>
-      </c>
-      <c r="B35" s="68" t="s">
+      <c r="C47" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47" s="57"/>
+      <c r="E47" s="18">
+        <v>43783</v>
+      </c>
+      <c r="F47" s="1">
+        <v>5</v>
+      </c>
+      <c r="G47" s="10"/>
+      <c r="H47" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I47" s="3"/>
+    </row>
+    <row r="48" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="10">
+        <v>6</v>
+      </c>
+      <c r="B48" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="25"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="3"/>
-    </row>
-    <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="10">
-        <v>4</v>
-      </c>
-      <c r="B36" s="68" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" s="25"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="3"/>
-    </row>
-    <row r="37" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="9"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="5"/>
-    </row>
-    <row r="38" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="B38" s="67" t="s">
-        <v>16</v>
-      </c>
-      <c r="C38" s="69">
-        <f>SUM(F31:F37)</f>
-        <v>0</v>
-      </c>
-      <c r="D38" s="69"/>
-      <c r="E38" s="69"/>
-      <c r="F38" s="70"/>
-      <c r="G38" s="66" t="s">
-        <v>17</v>
-      </c>
-      <c r="H38" s="69">
-        <f>SUM(G31:G37)</f>
-        <v>0</v>
-      </c>
-      <c r="I38" s="70"/>
-    </row>
-    <row r="39" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D39" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="E39" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F39" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="G39" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="H39" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="I39" s="24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="10">
-        <v>5</v>
-      </c>
-      <c r="B40" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" s="25"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="15"/>
-    </row>
-    <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="10">
-        <v>5</v>
-      </c>
-      <c r="B41" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" s="25"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="15"/>
-    </row>
-    <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="10">
-        <v>5</v>
-      </c>
-      <c r="B42" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="C42" s="25"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="3"/>
-    </row>
-    <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="10">
-        <v>5</v>
-      </c>
-      <c r="B43" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="3"/>
-    </row>
-    <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="10">
-        <v>5</v>
-      </c>
-      <c r="B44" s="68" t="s">
-        <v>13</v>
-      </c>
-      <c r="C44" s="25"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="3"/>
-    </row>
-    <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="10">
-        <v>5</v>
-      </c>
-      <c r="B45" s="68" t="s">
-        <v>14</v>
-      </c>
-      <c r="C45" s="25"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="3"/>
-    </row>
-    <row r="46" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="9"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="5"/>
-    </row>
-    <row r="47" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="B47" s="67" t="s">
-        <v>16</v>
-      </c>
-      <c r="C47" s="69">
-        <f>SUM(F40:F46)</f>
-        <v>0</v>
-      </c>
-      <c r="D47" s="69"/>
-      <c r="E47" s="69"/>
-      <c r="F47" s="70"/>
-      <c r="G47" s="66" t="s">
-        <v>17</v>
-      </c>
-      <c r="H47" s="69">
-        <f>SUM(G40:G46)</f>
-        <v>0</v>
-      </c>
-      <c r="I47" s="70"/>
-    </row>
-    <row r="48" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B48" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="C48" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D48" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="E48" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F48" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="G48" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="H48" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="I48" s="24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C48" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" s="63" t="s">
+        <v>175</v>
+      </c>
+      <c r="E48" s="18">
+        <v>43784</v>
+      </c>
+      <c r="F48" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G48" s="10"/>
+      <c r="H48" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I48" s="3"/>
+    </row>
+    <row r="49" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="10">
         <v>6</v>
       </c>
       <c r="B49" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" s="63" t="s">
+        <v>176</v>
+      </c>
+      <c r="E49" s="18">
+        <v>43785</v>
+      </c>
+      <c r="F49" s="1">
+        <v>6</v>
+      </c>
+      <c r="G49" s="10"/>
+      <c r="H49" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I49" s="3"/>
+    </row>
+    <row r="50" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="9"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="59"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="5"/>
+    </row>
+    <row r="51" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" s="77">
+        <f>SUM(F44:F50)</f>
+        <v>30.5</v>
+      </c>
+      <c r="D51" s="77"/>
+      <c r="E51" s="77"/>
+      <c r="F51" s="78"/>
+      <c r="G51" s="66" t="s">
+        <v>17</v>
+      </c>
+      <c r="H51" s="77">
+        <f>SUM(G44:G50)</f>
+        <v>0</v>
+      </c>
+      <c r="I51" s="78"/>
+    </row>
+    <row r="52" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="10">
+        <v>7</v>
+      </c>
+      <c r="B52" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C49" s="25"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="15"/>
-    </row>
-    <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="10">
+      <c r="C52" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D52" s="69" t="s">
+        <v>177</v>
+      </c>
+      <c r="E52" s="18">
+        <v>43787</v>
+      </c>
+      <c r="F52" s="10">
         <v>6</v>
       </c>
-      <c r="B50" s="27" t="s">
+      <c r="G52" s="10"/>
+      <c r="H52" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I52" s="15"/>
+    </row>
+    <row r="53" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="10">
+        <v>7</v>
+      </c>
+      <c r="B53" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C50" s="25"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="15"/>
-    </row>
-    <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="10">
+      <c r="C53" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D53" s="56"/>
+      <c r="E53" s="18">
+        <v>43788</v>
+      </c>
+      <c r="F53" s="10">
+        <v>4</v>
+      </c>
+      <c r="G53" s="10"/>
+      <c r="H53" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I53" s="15"/>
+    </row>
+    <row r="54" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="10">
+        <v>7</v>
+      </c>
+      <c r="B54" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D54" s="57" t="s">
+        <v>178</v>
+      </c>
+      <c r="E54" s="18">
+        <v>43789</v>
+      </c>
+      <c r="F54" s="1">
+        <v>5</v>
+      </c>
+      <c r="G54" s="10"/>
+      <c r="H54" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I54" s="3"/>
+    </row>
+    <row r="55" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="10">
+        <v>7</v>
+      </c>
+      <c r="B55" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D55" s="57" t="s">
+        <v>178</v>
+      </c>
+      <c r="E55" s="18">
+        <v>43790</v>
+      </c>
+      <c r="F55" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="G55" s="10"/>
+      <c r="H55" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I55" s="3"/>
+    </row>
+    <row r="56" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="10">
+        <v>7</v>
+      </c>
+      <c r="B56" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D56" s="63" t="s">
+        <v>179</v>
+      </c>
+      <c r="E56" s="18">
+        <v>43791</v>
+      </c>
+      <c r="F56" s="1">
+        <v>5</v>
+      </c>
+      <c r="G56" s="10"/>
+      <c r="H56" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I56" s="3"/>
+    </row>
+    <row r="57" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="10">
+        <v>7</v>
+      </c>
+      <c r="B57" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D57" s="63" t="s">
+        <v>180</v>
+      </c>
+      <c r="E57" s="18">
+        <v>43792</v>
+      </c>
+      <c r="F57" s="1">
         <v>6</v>
       </c>
-      <c r="B51" s="27" t="s">
+      <c r="G57" s="10"/>
+      <c r="H57" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I57" s="3"/>
+    </row>
+    <row r="58" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="9"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="59"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="5"/>
+    </row>
+    <row r="59" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="B59" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="C59" s="77">
+        <f>SUM(F52:F58)</f>
+        <v>32.5</v>
+      </c>
+      <c r="D59" s="77"/>
+      <c r="E59" s="77"/>
+      <c r="F59" s="78"/>
+      <c r="G59" s="66" t="s">
+        <v>17</v>
+      </c>
+      <c r="H59" s="77">
+        <f>SUM(G52:G58)</f>
+        <v>0</v>
+      </c>
+      <c r="I59" s="78"/>
+    </row>
+    <row r="60" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="10">
+        <v>8</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D60" s="84" t="s">
+        <v>181</v>
+      </c>
+      <c r="E60" s="18">
+        <v>43794</v>
+      </c>
+      <c r="F60" s="10">
+        <v>6</v>
+      </c>
+      <c r="G60" s="10"/>
+      <c r="H60" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I60" s="15"/>
+    </row>
+    <row r="61" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="10">
+        <v>8</v>
+      </c>
+      <c r="B61" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D61" s="56"/>
+      <c r="E61" s="18">
+        <v>43795</v>
+      </c>
+      <c r="F61" s="10">
+        <v>4</v>
+      </c>
+      <c r="G61" s="10"/>
+      <c r="H61" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I61" s="15"/>
+    </row>
+    <row r="62" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="10">
+        <v>8</v>
+      </c>
+      <c r="B62" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C51" s="25"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="3"/>
-    </row>
-    <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="10">
+      <c r="C62" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D62" s="57" t="s">
+        <v>182</v>
+      </c>
+      <c r="E62" s="18">
+        <v>43796</v>
+      </c>
+      <c r="F62" s="1">
         <v>6</v>
       </c>
-      <c r="B52" s="27" t="s">
+      <c r="G62" s="10"/>
+      <c r="H62" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I62" s="3"/>
+    </row>
+    <row r="63" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="10">
+        <v>8</v>
+      </c>
+      <c r="B63" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C52" s="25"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="3"/>
-    </row>
-    <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="10">
+      <c r="C63" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D63" s="57" t="s">
+        <v>172</v>
+      </c>
+      <c r="E63" s="18">
+        <v>43797</v>
+      </c>
+      <c r="F63" s="1">
+        <v>4</v>
+      </c>
+      <c r="G63" s="10"/>
+      <c r="H63" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I63" s="3"/>
+    </row>
+    <row r="64" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="10">
+        <v>8</v>
+      </c>
+      <c r="B64" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C64" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D64" s="63" t="s">
+        <v>183</v>
+      </c>
+      <c r="E64" s="18">
+        <v>43798</v>
+      </c>
+      <c r="F64" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="G64" s="10"/>
+      <c r="H64" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I64" s="3"/>
+    </row>
+    <row r="65" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A65" s="10">
+        <v>8</v>
+      </c>
+      <c r="B65" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D65" s="63" t="s">
+        <v>184</v>
+      </c>
+      <c r="E65" s="18">
+        <v>43799</v>
+      </c>
+      <c r="F65" s="1">
         <v>6</v>
       </c>
-      <c r="B53" s="68" t="s">
+      <c r="G65" s="10"/>
+      <c r="H65" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I65" s="3"/>
+    </row>
+    <row r="66" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="85">
+        <v>8</v>
+      </c>
+      <c r="B66" s="11"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="59"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="5"/>
+    </row>
+    <row r="67" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="67">
+        <v>8</v>
+      </c>
+      <c r="B67" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67" s="77">
+        <f>SUM(F60:F66)</f>
+        <v>31.5</v>
+      </c>
+      <c r="D67" s="77"/>
+      <c r="E67" s="77"/>
+      <c r="F67" s="78"/>
+      <c r="G67" s="66" t="s">
+        <v>17</v>
+      </c>
+      <c r="H67" s="77">
+        <f>SUM(G60:G66)</f>
+        <v>0</v>
+      </c>
+      <c r="I67" s="78"/>
+    </row>
+    <row r="68" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="10">
+        <v>9</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D68" s="84" t="s">
+        <v>185</v>
+      </c>
+      <c r="E68" s="18">
+        <v>43801</v>
+      </c>
+      <c r="F68" s="10">
+        <v>6</v>
+      </c>
+      <c r="G68" s="10"/>
+      <c r="H68" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I68" s="15"/>
+    </row>
+    <row r="69" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="10">
+        <v>9</v>
+      </c>
+      <c r="B69" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C69" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D69" s="56"/>
+      <c r="E69" s="18">
+        <v>43802</v>
+      </c>
+      <c r="F69" s="10">
+        <v>4</v>
+      </c>
+      <c r="G69" s="10"/>
+      <c r="H69" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I69" s="15"/>
+    </row>
+    <row r="70" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="10">
+        <v>9</v>
+      </c>
+      <c r="B70" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D70" s="57" t="s">
+        <v>185</v>
+      </c>
+      <c r="E70" s="18">
+        <v>43803</v>
+      </c>
+      <c r="F70" s="1">
+        <v>6</v>
+      </c>
+      <c r="G70" s="10"/>
+      <c r="H70" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I70" s="3"/>
+    </row>
+    <row r="71" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="10">
+        <v>9</v>
+      </c>
+      <c r="B71" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C71" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D71" s="57" t="s">
+        <v>186</v>
+      </c>
+      <c r="E71" s="18">
+        <v>43804</v>
+      </c>
+      <c r="F71" s="1">
+        <v>4</v>
+      </c>
+      <c r="G71" s="10"/>
+      <c r="H71" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I71" s="3"/>
+    </row>
+    <row r="72" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="10">
+        <v>9</v>
+      </c>
+      <c r="B72" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C53" s="25"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="3"/>
-    </row>
-    <row r="54" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="10">
+      <c r="C72" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D72" s="63" t="s">
+        <v>187</v>
+      </c>
+      <c r="E72" s="18">
+        <v>43805</v>
+      </c>
+      <c r="F72" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="G72" s="10"/>
+      <c r="H72" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I72" s="3"/>
+    </row>
+    <row r="73" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A73" s="10">
+        <v>9</v>
+      </c>
+      <c r="B73" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D73" s="63" t="s">
+        <v>184</v>
+      </c>
+      <c r="E73" s="18">
+        <v>43806</v>
+      </c>
+      <c r="F73" s="1">
         <v>6</v>
       </c>
-      <c r="B54" s="68" t="s">
-        <v>14</v>
-      </c>
-      <c r="C54" s="25"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="7"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="3"/>
-    </row>
-    <row r="55" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="9"/>
-      <c r="B55" s="12"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="8"/>
-      <c r="G55" s="8"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="5"/>
-    </row>
-    <row r="56" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="B56" s="67" t="s">
+      <c r="G73" s="10"/>
+      <c r="H73" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I73" s="3"/>
+    </row>
+    <row r="74" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="85">
+        <v>9</v>
+      </c>
+      <c r="B74" s="11"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="59"/>
+      <c r="E74" s="16"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="9"/>
+      <c r="H74" s="14"/>
+      <c r="I74" s="5"/>
+    </row>
+    <row r="75" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="67">
+        <v>9</v>
+      </c>
+      <c r="B75" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C56" s="69">
-        <f>SUM(F49:F55)</f>
+      <c r="C75" s="77">
+        <f>SUM(F68:F74)</f>
+        <v>31.5</v>
+      </c>
+      <c r="D75" s="77"/>
+      <c r="E75" s="77"/>
+      <c r="F75" s="78"/>
+      <c r="G75" s="66" t="s">
+        <v>17</v>
+      </c>
+      <c r="H75" s="77">
+        <f>SUM(G68:G74)</f>
         <v>0</v>
       </c>
-      <c r="D56" s="69"/>
-      <c r="E56" s="69"/>
-      <c r="F56" s="70"/>
-      <c r="G56" s="66" t="s">
-        <v>17</v>
-      </c>
-      <c r="H56" s="69">
-        <f>SUM(G49:G55)</f>
-        <v>0</v>
-      </c>
-      <c r="I56" s="70"/>
+      <c r="I75" s="78"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="C56:F56"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="H47:I47"/>
+  <mergeCells count="19">
+    <mergeCell ref="C59:F59"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="C67:F67"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="C75:F75"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="H43:I43"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="C11:F11"/>
     <mergeCell ref="H11:I11"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="H51:I51"/>
   </mergeCells>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C19 C28 C37 C46 C55" xr:uid="{6E08E741-C8C7-4210-9264-8F4FCE40EB21}">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C18 C26 C34 C42 C50 C58 C66 C74" xr:uid="{37F695A9-FAA1-4B0C-BCF8-EDBE86D67943}">
       <formula1>"Project Management, Requirement, Architecture and Desgin, Implementation, Testing, Training, Meetting Customer, Meetting Mentor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C9 C13:C18 C22:C27 C31:C36 C40:C45 C49:C54" xr:uid="{FEE62105-1E1C-408F-82C0-11D2CE7772AA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C9 C12:C17 C20:C25 C28:C33 C36:C41 C44:C49 C52:C57 C61:C65 C69:C73" xr:uid="{4DC3D9AA-11CE-4711-9ED3-197750CC8F84}">
       <formula1>"Project Management, Requirement, Architecture and Desgin, Implementation, Testing, Training, Meetting Customer, Meeting Mentor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H10 H13:H19 H22:H28 H31:H37 H40:H46 H49:H55" xr:uid="{E64829C6-8241-4F40-B7F6-06026AC59D56}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H10 H12:H18 H20:H26 H28:H34 H36:H42 H44:H50 H68:H74 H60:H66 H52:H58" xr:uid="{2584A001-B154-4F5B-91E6-3C188ADCF05D}">
       <formula1>"Done,Inprogress "</formula1>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 B12" xr:uid="{33954315-0CBA-47B2-A2B7-73FE39F329C3}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{EBEBF163-72C9-402A-BB5E-65147965157F}">
       <formula1>B4</formula1>
       <formula2>B10</formula2>
-    </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21" xr:uid="{6622A24D-4DEB-4C6F-A379-E82812C473F0}">
-      <formula1>#REF!</formula1>
-      <formula2>B27</formula2>
-    </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30 B39 B48" xr:uid="{CE3F35D2-C816-4009-8BAB-85DA53F798DE}">
-      <formula1>#REF!</formula1>
-      <formula2>B35</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>